<commit_message>
added initial size data
</commit_message>
<xml_diff>
--- a/data/loggers/logger_metadata.xlsx
+++ b/data/loggers/logger_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/manchester-hardening/data/loggers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435C0846-8DCE-8D41-92AE-C7616C624BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5D8FBC-1FF5-3A4D-B29C-9552E5CA747F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{910C5C9C-1199-2F4F-A6BD-E003E55895D4}"/>
+    <workbookView xWindow="1500" yWindow="1320" windowWidth="13980" windowHeight="16300" xr2:uid="{910C5C9C-1199-2F4F-A6BD-E003E55895D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>logger</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>header</t>
+  </si>
+  <si>
+    <t>field_tag</t>
+  </si>
+  <si>
+    <t>R008</t>
+  </si>
+  <si>
+    <t>G058</t>
+  </si>
+  <si>
+    <t>R013</t>
+  </si>
+  <si>
+    <t>B028</t>
   </si>
 </sst>
 </file>
@@ -425,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026AE326-2012-A844-AB6A-692D667495E5}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,8 +461,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>22105353</v>
       </c>
@@ -460,8 +478,11 @@
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>22105354</v>
       </c>
@@ -474,8 +495,11 @@
       <c r="D3">
         <v>2</v>
       </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>22105356</v>
       </c>
@@ -488,8 +512,11 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>22105358</v>
       </c>
@@ -501,6 +528,9 @@
       </c>
       <c r="D5">
         <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>